<commit_message>
sửa bảng phân công
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -258,9 +258,6 @@
     <t>Quản lý lớp</t>
   </si>
   <si>
-    <t>nhập và sửa điểm</t>
-  </si>
-  <si>
     <t>Quản lý điểm theo bộ môn</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>thêm ,xóa ,sửa học sinh</t>
+  </si>
+  <si>
+    <t>nhập và sửa điểm môn học</t>
   </si>
 </sst>
 </file>
@@ -538,6 +538,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,9 +596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,45 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -926,122 +926,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="23" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="21" customHeight="1">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="75" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A6" s="44"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="46" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="44"/>
-      <c r="B7" s="30" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="44"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:5" ht="33" customHeight="1">
-      <c r="A9" s="44"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="52.5" customHeight="1">
-      <c r="A10" s="44"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" ht="52.5" customHeight="1">
-      <c r="A11" s="45"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" s="16" customFormat="1" ht="24.75" customHeight="1">
       <c r="A13" s="4" t="s">
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="49.5">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="46" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1078,7 +1078,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="49.5">
-      <c r="A15" s="34"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="49.5">
-      <c r="A16" s="34"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
@@ -1108,7 +1108,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="49.5">
-      <c r="A17" s="34"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
@@ -1123,7 +1123,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="66.75" customHeight="1">
-      <c r="A18" s="35"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1145,7 @@
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="41" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -1160,7 +1160,7 @@
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="27"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="27"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="12" t="s">
         <v>55</v>
       </c>
@@ -1184,14 +1184,14 @@
       <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="41" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1204,7 +1204,7 @@
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="27"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="6" t="s">
         <v>28</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:11" ht="49.5">
-      <c r="A26" s="27"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="6" t="s">
         <v>27</v>
       </c>
@@ -1232,7 +1232,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="66">
-      <c r="A27" s="27"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="12" t="s">
         <v>75</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="66">
-      <c r="A28" s="27"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="12" t="s">
         <v>25</v>
       </c>
@@ -1258,9 +1258,9 @@
       </c>
     </row>
     <row r="29" spans="1:11" s="5" customFormat="1" ht="33">
-      <c r="A29" s="27"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>74</v>
@@ -1283,7 +1283,7 @@
         <v>76</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="7">
         <v>3</v>
@@ -1292,11 +1292,11 @@
         <v>71</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="5" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="42" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -1306,10 +1306,10 @@
         <v>2</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1319,7 +1319,7 @@
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" s="5" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A32" s="28"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="12" t="s">
         <v>77</v>
       </c>
@@ -1327,10 +1327,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1340,18 +1340,18 @@
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" s="5" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A33" s="28"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="24">
         <v>2</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1361,7 +1361,7 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" s="5" customFormat="1" ht="27" customHeight="1">
-      <c r="A34" s="28"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="12" t="s">
         <v>79</v>
       </c>
@@ -1369,10 +1369,10 @@
         <v>3</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1382,7 +1382,7 @@
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="39" customHeight="1">
-      <c r="A35" s="28"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="12" t="s">
         <v>67</v>
       </c>
@@ -1393,11 +1393,11 @@
         <v>72</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A36" s="28"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="12" t="s">
         <v>68</v>
       </c>
@@ -1408,7 +1408,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="66">
-      <c r="A37" s="28"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="12" t="s">
         <v>33</v>
       </c>
@@ -1423,7 +1423,7 @@
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="28"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="12" t="s">
         <v>31</v>
       </c>
@@ -1438,7 +1438,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="99">
-      <c r="A39" s="28"/>
+      <c r="A39" s="42"/>
       <c r="B39" s="12" t="s">
         <v>37</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="33">
-      <c r="A40" s="28"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="12" t="s">
         <v>35</v>
       </c>
@@ -1576,13 +1576,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="C6:E6"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A24:A29"/>
     <mergeCell ref="A31:A40"/>
@@ -1597,6 +1590,13 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>